<commit_message>
tested environmentvars class, need to work on getting past 5 candles and assigning their colors.
</commit_message>
<xml_diff>
--- a/trading-signaller/main_sheet.xlsx
+++ b/trading-signaller/main_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wen_z\Documents\GitHub\trading-signaller\trading-signaller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07398F03-3BC1-4D87-944D-523C9E4588B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D195F8FF-C7BF-4CBE-B6FE-4D780F8A6D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView showSheetTabs="0" xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="63">
   <si>
     <t>-5
 H/L/CL</t>
@@ -226,6 +226,9 @@
   </si>
   <si>
     <t>12H</t>
+  </si>
+  <si>
+    <t>0.70594 / 0.70010 / 0.70171</t>
   </si>
 </sst>
 </file>
@@ -749,6 +752,21 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -767,6 +785,24 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -790,39 +826,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1114,14 +1117,14 @@
   </sheetPr>
   <dimension ref="A1:AF38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="52" zoomScaleNormal="52" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.26953125" defaultRowHeight="40" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="23.26953125" style="1"/>
-    <col min="3" max="3" width="15" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.90625" style="1" customWidth="1"/>
     <col min="4" max="4" width="36.1796875" style="1" customWidth="1"/>
     <col min="5" max="5" width="15" style="1" customWidth="1"/>
     <col min="6" max="6" width="36.1796875" style="1" customWidth="1"/>
@@ -1151,38 +1154,38 @@
     <row r="1" spans="1:32" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="55"/>
-      <c r="E1" s="58" t="s">
+      <c r="D1" s="48"/>
+      <c r="E1" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="58"/>
-      <c r="G1" s="42" t="s">
+      <c r="F1" s="51"/>
+      <c r="G1" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="42"/>
-      <c r="I1" s="44" t="s">
+      <c r="H1" s="53"/>
+      <c r="I1" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="44"/>
-      <c r="K1" s="46" t="s">
+      <c r="J1" s="55"/>
+      <c r="K1" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="L1" s="46"/>
-      <c r="M1" s="48" t="s">
+      <c r="L1" s="57"/>
+      <c r="M1" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="N1" s="48"/>
-      <c r="O1" s="50" t="s">
+      <c r="N1" s="59"/>
+      <c r="O1" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="52" t="s">
+      <c r="P1" s="37"/>
+      <c r="Q1" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="52"/>
+      <c r="R1" s="39"/>
       <c r="S1" s="34"/>
       <c r="T1" s="34"/>
       <c r="U1" s="34"/>
@@ -1201,22 +1204,22 @@
     <row r="2" spans="1:32" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="53"/>
-      <c r="R2" s="53"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
       <c r="S2" s="34"/>
       <c r="T2" s="34"/>
       <c r="U2" s="34"/>
@@ -1233,56 +1236,56 @@
       <c r="AF2" s="12"/>
     </row>
     <row r="3" spans="1:32" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="37"/>
+      <c r="B3" s="42"/>
       <c r="C3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="D3" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="60" t="s">
+      <c r="G3" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="60" t="s">
+      <c r="I3" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="J3" s="60" t="s">
+      <c r="K3" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="L3" s="60" t="s">
+      <c r="M3" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="N3" s="60" t="s">
+      <c r="O3" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="O3" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="P3" s="60" t="s">
-        <v>21</v>
-      </c>
       <c r="Q3" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="R3" s="60" t="s">
+      <c r="R3" s="36" t="s">
         <v>21</v>
       </c>
       <c r="S3" s="35"/>
@@ -1301,8 +1304,8 @@
       <c r="AF3" s="8"/>
     </row>
     <row r="4" spans="1:32" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="38"/>
-      <c r="B4" s="39"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="26" t="s">
         <v>2</v>
       </c>
@@ -1367,8 +1370,8 @@
       <c r="AF4" s="10"/>
     </row>
     <row r="5" spans="1:32" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="38"/>
-      <c r="B5" s="39"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="44"/>
       <c r="C5" s="26" t="s">
         <v>3</v>
       </c>
@@ -1439,8 +1442,8 @@
       </c>
     </row>
     <row r="6" spans="1:32" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="38"/>
-      <c r="B6" s="39"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="44"/>
       <c r="C6" s="26" t="s">
         <v>4</v>
       </c>
@@ -1511,8 +1514,8 @@
       </c>
     </row>
     <row r="7" spans="1:32" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="38"/>
-      <c r="B7" s="39"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="44"/>
       <c r="C7" s="26" t="s">
         <v>5</v>
       </c>
@@ -1577,8 +1580,8 @@
       <c r="AF7" s="8"/>
     </row>
     <row r="8" spans="1:32" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="40"/>
-      <c r="B8" s="41"/>
+      <c r="A8" s="45"/>
+      <c r="B8" s="46"/>
       <c r="C8" s="29" t="s">
         <v>0</v>
       </c>
@@ -1643,56 +1646,56 @@
       <c r="AF8" s="10"/>
     </row>
     <row r="9" spans="1:32" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="37"/>
+      <c r="B9" s="42"/>
       <c r="C9" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="60" t="s">
+      <c r="D9" s="36" t="s">
         <v>27</v>
       </c>
       <c r="E9" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="60" t="s">
+      <c r="F9" s="36" t="s">
         <v>27</v>
       </c>
       <c r="G9" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="60" t="s">
+      <c r="H9" s="36" t="s">
         <v>27</v>
       </c>
       <c r="I9" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="J9" s="60" t="s">
+      <c r="J9" s="36" t="s">
         <v>27</v>
       </c>
       <c r="K9" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="L9" s="60" t="s">
+      <c r="L9" s="36" t="s">
         <v>27</v>
       </c>
       <c r="M9" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="N9" s="60" t="s">
+      <c r="N9" s="36" t="s">
         <v>27</v>
       </c>
       <c r="O9" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="P9" s="60" t="s">
+      <c r="P9" s="36" t="s">
         <v>27</v>
       </c>
       <c r="Q9" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="R9" s="60" t="s">
+      <c r="R9" s="36" t="s">
         <v>27</v>
       </c>
       <c r="S9" s="35"/>
@@ -1717,8 +1720,8 @@
       </c>
     </row>
     <row r="10" spans="1:32" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="38"/>
-      <c r="B10" s="39"/>
+      <c r="A10" s="43"/>
+      <c r="B10" s="44"/>
       <c r="C10" s="26" t="s">
         <v>2</v>
       </c>
@@ -1789,8 +1792,8 @@
       </c>
     </row>
     <row r="11" spans="1:32" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="38"/>
-      <c r="B11" s="39"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="44"/>
       <c r="C11" s="26" t="s">
         <v>3</v>
       </c>
@@ -1855,8 +1858,8 @@
       <c r="AF11" s="8"/>
     </row>
     <row r="12" spans="1:32" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="38"/>
-      <c r="B12" s="39"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="44"/>
       <c r="C12" s="26" t="s">
         <v>4</v>
       </c>
@@ -1921,8 +1924,8 @@
       <c r="AF12" s="10"/>
     </row>
     <row r="13" spans="1:32" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="38"/>
-      <c r="B13" s="39"/>
+      <c r="A13" s="43"/>
+      <c r="B13" s="44"/>
       <c r="C13" s="26" t="s">
         <v>5</v>
       </c>
@@ -1993,8 +1996,8 @@
       </c>
     </row>
     <row r="14" spans="1:32" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="40"/>
-      <c r="B14" s="41"/>
+      <c r="A14" s="45"/>
+      <c r="B14" s="46"/>
       <c r="C14" s="29" t="s">
         <v>0</v>
       </c>
@@ -2065,56 +2068,56 @@
       </c>
     </row>
     <row r="15" spans="1:32" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="37"/>
+      <c r="B15" s="42"/>
       <c r="C15" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="60" t="s">
+      <c r="D15" s="36" t="s">
         <v>33</v>
       </c>
       <c r="E15" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="F15" s="60" t="s">
+      <c r="F15" s="36" t="s">
         <v>33</v>
       </c>
       <c r="G15" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="H15" s="60" t="s">
+      <c r="H15" s="36" t="s">
         <v>33</v>
       </c>
       <c r="I15" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="J15" s="60" t="s">
+      <c r="J15" s="36" t="s">
         <v>33</v>
       </c>
       <c r="K15" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="L15" s="60" t="s">
+      <c r="L15" s="36" t="s">
         <v>33</v>
       </c>
       <c r="M15" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="N15" s="60" t="s">
+      <c r="N15" s="36" t="s">
         <v>33</v>
       </c>
       <c r="O15" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="P15" s="60" t="s">
+      <c r="P15" s="36" t="s">
         <v>33</v>
       </c>
       <c r="Q15" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="R15" s="60" t="s">
+      <c r="R15" s="36" t="s">
         <v>33</v>
       </c>
       <c r="S15" s="35"/>
@@ -2133,8 +2136,8 @@
       <c r="AF15" s="8"/>
     </row>
     <row r="16" spans="1:32" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="38"/>
-      <c r="B16" s="39"/>
+      <c r="A16" s="43"/>
+      <c r="B16" s="44"/>
       <c r="C16" s="26" t="s">
         <v>2</v>
       </c>
@@ -2199,8 +2202,8 @@
       <c r="AF16" s="10"/>
     </row>
     <row r="17" spans="1:32" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="38"/>
-      <c r="B17" s="39"/>
+      <c r="A17" s="43"/>
+      <c r="B17" s="44"/>
       <c r="C17" s="26" t="s">
         <v>3</v>
       </c>
@@ -2271,8 +2274,8 @@
       </c>
     </row>
     <row r="18" spans="1:32" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="38"/>
-      <c r="B18" s="39"/>
+      <c r="A18" s="43"/>
+      <c r="B18" s="44"/>
       <c r="C18" s="26" t="s">
         <v>4</v>
       </c>
@@ -2343,8 +2346,8 @@
       </c>
     </row>
     <row r="19" spans="1:32" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="38"/>
-      <c r="B19" s="39"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="44"/>
       <c r="C19" s="26" t="s">
         <v>5</v>
       </c>
@@ -2409,8 +2412,8 @@
       <c r="AF19" s="8"/>
     </row>
     <row r="20" spans="1:32" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="40"/>
-      <c r="B20" s="41"/>
+      <c r="A20" s="45"/>
+      <c r="B20" s="46"/>
       <c r="C20" s="29" t="s">
         <v>0</v>
       </c>
@@ -2475,56 +2478,56 @@
       <c r="AF20" s="10"/>
     </row>
     <row r="21" spans="1:32" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="36" t="s">
+      <c r="A21" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="37"/>
+      <c r="B21" s="42"/>
       <c r="C21" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="60" t="s">
+      <c r="D21" s="36" t="s">
         <v>39</v>
       </c>
       <c r="E21" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="F21" s="60" t="s">
+      <c r="F21" s="36" t="s">
         <v>39</v>
       </c>
       <c r="G21" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="H21" s="60" t="s">
+      <c r="H21" s="36" t="s">
         <v>39</v>
       </c>
       <c r="I21" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="J21" s="60" t="s">
+      <c r="J21" s="36" t="s">
         <v>39</v>
       </c>
       <c r="K21" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="L21" s="60" t="s">
+      <c r="L21" s="36" t="s">
         <v>39</v>
       </c>
       <c r="M21" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="N21" s="60" t="s">
+      <c r="N21" s="36" t="s">
         <v>39</v>
       </c>
       <c r="O21" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="P21" s="60" t="s">
+      <c r="P21" s="36" t="s">
         <v>39</v>
       </c>
       <c r="Q21" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="R21" s="60" t="s">
+      <c r="R21" s="36" t="s">
         <v>39</v>
       </c>
       <c r="S21" s="35"/>
@@ -2549,8 +2552,8 @@
       </c>
     </row>
     <row r="22" spans="1:32" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="38"/>
-      <c r="B22" s="39"/>
+      <c r="A22" s="43"/>
+      <c r="B22" s="44"/>
       <c r="C22" s="26" t="s">
         <v>2</v>
       </c>
@@ -2621,8 +2624,8 @@
       </c>
     </row>
     <row r="23" spans="1:32" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="38"/>
-      <c r="B23" s="39"/>
+      <c r="A23" s="43"/>
+      <c r="B23" s="44"/>
       <c r="C23" s="26" t="s">
         <v>3</v>
       </c>
@@ -2687,8 +2690,8 @@
       <c r="AF23" s="8"/>
     </row>
     <row r="24" spans="1:32" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="38"/>
-      <c r="B24" s="39"/>
+      <c r="A24" s="43"/>
+      <c r="B24" s="44"/>
       <c r="C24" s="26" t="s">
         <v>4</v>
       </c>
@@ -2753,8 +2756,8 @@
       <c r="AF24" s="10"/>
     </row>
     <row r="25" spans="1:32" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="38"/>
-      <c r="B25" s="39"/>
+      <c r="A25" s="43"/>
+      <c r="B25" s="44"/>
       <c r="C25" s="26" t="s">
         <v>5</v>
       </c>
@@ -2825,8 +2828,8 @@
       </c>
     </row>
     <row r="26" spans="1:32" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="40"/>
-      <c r="B26" s="41"/>
+      <c r="A26" s="45"/>
+      <c r="B26" s="46"/>
       <c r="C26" s="29" t="s">
         <v>0</v>
       </c>
@@ -2897,56 +2900,56 @@
       </c>
     </row>
     <row r="27" spans="1:32" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="37"/>
+      <c r="B27" s="42"/>
       <c r="C27" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="60" t="s">
+      <c r="D27" s="36" t="s">
         <v>45</v>
       </c>
       <c r="E27" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="F27" s="60" t="s">
+      <c r="F27" s="36" t="s">
         <v>45</v>
       </c>
       <c r="G27" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="H27" s="60" t="s">
+      <c r="H27" s="36" t="s">
         <v>45</v>
       </c>
       <c r="I27" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="J27" s="60" t="s">
+      <c r="J27" s="36" t="s">
         <v>45</v>
       </c>
       <c r="K27" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="L27" s="60" t="s">
+      <c r="L27" s="36" t="s">
         <v>45</v>
       </c>
       <c r="M27" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="N27" s="60" t="s">
+      <c r="N27" s="36" t="s">
         <v>45</v>
       </c>
       <c r="O27" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="P27" s="60" t="s">
+      <c r="P27" s="36" t="s">
         <v>45</v>
       </c>
       <c r="Q27" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="R27" s="60" t="s">
+      <c r="R27" s="36" t="s">
         <v>45</v>
       </c>
       <c r="S27" s="35"/>
@@ -2965,8 +2968,8 @@
       <c r="AF27" s="8"/>
     </row>
     <row r="28" spans="1:32" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="38"/>
-      <c r="B28" s="39"/>
+      <c r="A28" s="43"/>
+      <c r="B28" s="44"/>
       <c r="C28" s="26" t="s">
         <v>2</v>
       </c>
@@ -3031,8 +3034,8 @@
       <c r="AF28" s="10"/>
     </row>
     <row r="29" spans="1:32" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="38"/>
-      <c r="B29" s="39"/>
+      <c r="A29" s="43"/>
+      <c r="B29" s="44"/>
       <c r="C29" s="26" t="s">
         <v>3</v>
       </c>
@@ -3103,8 +3106,8 @@
       </c>
     </row>
     <row r="30" spans="1:32" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="38"/>
-      <c r="B30" s="39"/>
+      <c r="A30" s="43"/>
+      <c r="B30" s="44"/>
       <c r="C30" s="26" t="s">
         <v>4</v>
       </c>
@@ -3175,8 +3178,8 @@
       </c>
     </row>
     <row r="31" spans="1:32" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="38"/>
-      <c r="B31" s="39"/>
+      <c r="A31" s="43"/>
+      <c r="B31" s="44"/>
       <c r="C31" s="26" t="s">
         <v>5</v>
       </c>
@@ -3227,8 +3230,8 @@
       </c>
     </row>
     <row r="32" spans="1:32" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="40"/>
-      <c r="B32" s="41"/>
+      <c r="A32" s="45"/>
+      <c r="B32" s="46"/>
       <c r="C32" s="29" t="s">
         <v>0</v>
       </c>
@@ -3279,62 +3282,62 @@
       </c>
     </row>
     <row r="33" spans="1:18" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="36" t="s">
+      <c r="A33" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B33" s="37"/>
+      <c r="B33" s="42"/>
       <c r="C33" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D33" s="60" t="s">
+      <c r="D33" s="36" t="s">
         <v>51</v>
       </c>
       <c r="E33" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="F33" s="60" t="s">
+      <c r="F33" s="36" t="s">
         <v>51</v>
       </c>
       <c r="G33" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="H33" s="60" t="s">
+      <c r="H33" s="36" t="s">
         <v>51</v>
       </c>
       <c r="I33" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="J33" s="60" t="s">
+      <c r="J33" s="36" t="s">
         <v>51</v>
       </c>
       <c r="K33" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="L33" s="60" t="s">
+      <c r="L33" s="36" t="s">
         <v>51</v>
       </c>
       <c r="M33" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="N33" s="60" t="s">
+      <c r="N33" s="36" t="s">
         <v>51</v>
       </c>
       <c r="O33" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="P33" s="60" t="s">
+      <c r="P33" s="36" t="s">
         <v>51</v>
       </c>
       <c r="Q33" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="R33" s="60" t="s">
+      <c r="R33" s="36" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:18" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="38"/>
-      <c r="B34" s="39"/>
+      <c r="A34" s="43"/>
+      <c r="B34" s="44"/>
       <c r="C34" s="26" t="s">
         <v>2</v>
       </c>
@@ -3385,8 +3388,8 @@
       </c>
     </row>
     <row r="35" spans="1:18" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="38"/>
-      <c r="B35" s="39"/>
+      <c r="A35" s="43"/>
+      <c r="B35" s="44"/>
       <c r="C35" s="26" t="s">
         <v>3</v>
       </c>
@@ -3437,8 +3440,8 @@
       </c>
     </row>
     <row r="36" spans="1:18" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="38"/>
-      <c r="B36" s="39"/>
+      <c r="A36" s="43"/>
+      <c r="B36" s="44"/>
       <c r="C36" s="26" t="s">
         <v>4</v>
       </c>
@@ -3489,8 +3492,8 @@
       </c>
     </row>
     <row r="37" spans="1:18" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="38"/>
-      <c r="B37" s="39"/>
+      <c r="A37" s="43"/>
+      <c r="B37" s="44"/>
       <c r="C37" s="26" t="s">
         <v>5</v>
       </c>
@@ -3541,8 +3544,8 @@
       </c>
     </row>
     <row r="38" spans="1:18" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="40"/>
-      <c r="B38" s="41"/>
+      <c r="A38" s="45"/>
+      <c r="B38" s="46"/>
       <c r="C38" s="29" t="s">
         <v>0</v>
       </c>
@@ -3594,11 +3597,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="O1:P2"/>
-    <mergeCell ref="Q1:R2"/>
-    <mergeCell ref="A3:B8"/>
-    <mergeCell ref="C1:D2"/>
-    <mergeCell ref="E1:F2"/>
     <mergeCell ref="A33:B38"/>
     <mergeCell ref="G1:H2"/>
     <mergeCell ref="I1:J2"/>
@@ -3608,6 +3606,11 @@
     <mergeCell ref="A15:B20"/>
     <mergeCell ref="A21:B26"/>
     <mergeCell ref="A27:B32"/>
+    <mergeCell ref="O1:P2"/>
+    <mergeCell ref="Q1:R2"/>
+    <mergeCell ref="A3:B8"/>
+    <mergeCell ref="C1:D2"/>
+    <mergeCell ref="E1:F2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>